<commit_message>
fix annex_a end_to_end test
</commit_message>
<xml_diff>
--- a/liiatools/annex_a_pipeline/spec/samples/Annex_A.xlsx
+++ b/liiatools/annex_a_pipeline/spec/samples/Annex_A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://socialfinanceltd-my.sharepoint.com/personal/michael_hanks_socialfinance_org_uk/Documents/Desktop/Fake LDS 2/LA folders/Bromley/Annex A/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://socialfinanceltd-my.sharepoint.com/personal/patrick_troy_socialfinance_org_uk/Documents/Documents/GitHub/liia-tools/liiatools/annex_a_pipeline/spec/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{E4A36D23-2127-4ACC-8656-C2301DD801F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82872814-11A8-49E3-AF6E-BD0458400AD1}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{E4A36D23-2127-4ACC-8656-C2301DD801F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79561DC2-6496-4C9B-AF65-A18B787CCB6A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{16B5CE67-0781-4575-8251-1FD3DD33A5AC}"/>
+    <workbookView xWindow="3780" yWindow="3825" windowWidth="28800" windowHeight="15345" activeTab="9" xr2:uid="{16B5CE67-0781-4575-8251-1FD3DD33A5AC}"/>
   </bookViews>
   <sheets>
     <sheet name="List 1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="195">
   <si>
     <t>Child Unique ID</t>
   </si>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t>Date Placed for Adoption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Adoption Order </t>
   </si>
   <si>
     <t>Date of Decision that Child Should No Longer be Placed for Adoption</t>
@@ -671,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,7 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1024,18 +1020,18 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>9212044</v>
       </c>
@@ -1081,7 +1077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11973218</v>
       </c>
@@ -1102,7 +1098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>6217392</v>
       </c>
@@ -1125,7 +1121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>16248829</v>
       </c>
@@ -1148,7 +1144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>13981739</v>
       </c>
@@ -1180,13 +1176,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CADCE9-2BB8-459E-853E-7D6568F621BA}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1224,19 +1223,19 @@
         <v>171</v>
       </c>
       <c r="M1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N1" t="s">
         <v>172</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>173</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>174</v>
       </c>
-      <c r="P1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7961370</v>
       </c>
@@ -1258,7 +1257,7 @@
       <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="9">
         <v>40031</v>
       </c>
       <c r="I2" s="3">
@@ -1278,12 +1277,11 @@
         <v>40051</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" si="0"/>
         <v>40056</v>
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10414520</v>
       </c>
@@ -1305,7 +1303,7 @@
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>40031</v>
       </c>
       <c r="I3" s="3">
@@ -1325,12 +1323,11 @@
         <v>40051</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" si="1"/>
         <v>40056</v>
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>13782635</v>
       </c>
@@ -1352,7 +1349,7 @@
       <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>41894</v>
       </c>
       <c r="I4" s="3">
@@ -1372,7 +1369,6 @@
         <v>41914</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="1"/>
         <v>41919</v>
       </c>
       <c r="N4" s="3">
@@ -1380,10 +1376,10 @@
         <v>41924</v>
       </c>
       <c r="O4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4939073</v>
       </c>
@@ -1405,7 +1401,7 @@
       <c r="G5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>40233</v>
       </c>
       <c r="I5" s="3">
@@ -1425,12 +1421,11 @@
         <v>40253</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="1"/>
         <v>40258</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6102196</v>
       </c>
@@ -1452,7 +1447,7 @@
       <c r="G6" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>39743</v>
       </c>
       <c r="I6" s="3">
@@ -1472,7 +1467,6 @@
         <v>39763</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="1"/>
         <v>39768</v>
       </c>
       <c r="N6" s="3"/>
@@ -1486,13 +1480,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF2FA9E-C43C-4545-B42A-2CE1057450AF}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
         <v>165</v>
@@ -1504,52 +1503,52 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
         <v>178</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>179</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>180</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>181</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>182</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>183</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>184</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>185</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>186</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>187</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>188</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>190</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>191</v>
       </c>
-      <c r="S1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7105179</v>
       </c>
@@ -1568,51 +1567,51 @@
       <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <v>40031</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <f>G2+13</f>
         <v>40044</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <f t="shared" ref="I2:O2" si="0">H2+13</f>
         <v>40057</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <f t="shared" si="0"/>
         <v>40070</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="12">
         <f t="shared" si="0"/>
         <v>40083</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="12">
         <f t="shared" si="0"/>
         <v>40096</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="12">
         <f t="shared" si="0"/>
         <v>40109</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <f t="shared" si="0"/>
         <v>40122</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="12">
         <f t="shared" si="0"/>
         <v>40135</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="12">
         <f>O2+3</f>
         <v>40138</v>
       </c>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10898578</v>
       </c>
@@ -1631,51 +1630,51 @@
       <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>40031</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <f t="shared" ref="H3:O6" si="1">G3+13</f>
         <v>40044</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <f t="shared" si="1"/>
         <v>40057</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <f t="shared" si="1"/>
         <v>40070</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="12">
         <f t="shared" si="1"/>
         <v>40083</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="12">
         <f t="shared" si="1"/>
         <v>40096</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="12">
         <f t="shared" si="1"/>
         <v>40109</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="12">
         <f t="shared" si="1"/>
         <v>40122</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="12">
         <f t="shared" si="1"/>
         <v>40135</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="12">
         <f t="shared" ref="Q3:Q6" si="2">O3+3</f>
         <v>40138</v>
       </c>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7131857</v>
       </c>
@@ -1694,51 +1693,51 @@
       <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>41894</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <f t="shared" si="1"/>
         <v>41907</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <f t="shared" si="1"/>
         <v>41920</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <f t="shared" si="1"/>
         <v>41933</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <f t="shared" si="1"/>
         <v>41946</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="12">
         <f t="shared" si="1"/>
         <v>41959</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="12">
         <f t="shared" si="1"/>
         <v>41972</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="12">
         <f t="shared" si="1"/>
         <v>41985</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="12">
         <f t="shared" si="1"/>
         <v>41998</v>
       </c>
       <c r="P4">
         <v>1</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="12">
         <f t="shared" si="2"/>
         <v>42001</v>
       </c>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R4" s="12"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>11340940</v>
       </c>
@@ -1757,49 +1756,49 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>40233</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <f t="shared" si="1"/>
         <v>40246</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f t="shared" si="1"/>
         <v>40259</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <f t="shared" si="1"/>
         <v>40272</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <f t="shared" si="1"/>
         <v>40285</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <f t="shared" si="1"/>
         <v>40298</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <f t="shared" si="1"/>
         <v>40311</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="12">
         <f t="shared" si="1"/>
         <v>40324</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <f t="shared" si="1"/>
         <v>40337</v>
       </c>
       <c r="P5">
         <v>1</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="12">
         <f t="shared" si="2"/>
         <v>40340</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="12">
         <f>Q5+3</f>
         <v>40343</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2937497</v>
       </c>
@@ -1826,49 +1825,49 @@
       <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>39743</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <f t="shared" si="1"/>
         <v>39756</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <f t="shared" si="1"/>
         <v>39769</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <f t="shared" si="1"/>
         <v>39782</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <f t="shared" si="1"/>
         <v>39795</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="12">
         <f t="shared" si="1"/>
         <v>39808</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="12">
         <f t="shared" si="1"/>
         <v>39821</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="12">
         <f t="shared" si="1"/>
         <v>39834</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <f t="shared" si="1"/>
         <v>39847</v>
       </c>
       <c r="P6">
         <v>3</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="12">
         <f t="shared" si="2"/>
         <v>39850</v>
       </c>
-      <c r="R6" s="13"/>
+      <c r="R6" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1883,19 +1882,19 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>612306</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>6890906</v>
       </c>
@@ -1973,7 +1972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8778646</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10600594</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>16216178</v>
       </c>
@@ -2064,22 +2063,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2095,26 +2094,26 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>6537810</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4653765</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>997679</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>14007367</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10897459</v>
       </c>
@@ -2289,7 +2288,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11096583</v>
       </c>
@@ -2337,23 +2336,23 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2390,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10692868</v>
       </c>
@@ -2413,7 +2412,7 @@
       <c r="G2" s="3">
         <v>43601</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="3">
@@ -2429,7 +2428,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>15221387</v>
       </c>
@@ -2451,7 +2450,7 @@
       <c r="G3" s="3">
         <v>43768</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I3" s="3">
@@ -2467,7 +2466,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12590177</v>
       </c>
@@ -2489,7 +2488,7 @@
       <c r="G4" s="3">
         <v>43825</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I4" s="3">
@@ -2505,7 +2504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>15765513</v>
       </c>
@@ -2527,7 +2526,7 @@
       <c r="G5" s="3">
         <v>43887</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I5" s="3">
@@ -2543,7 +2542,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>12012513</v>
       </c>
@@ -2565,7 +2564,7 @@
       <c r="G6" s="3">
         <v>43887</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="3">
@@ -2594,25 +2593,25 @@
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2644,10 +2643,10 @@
         <v>57</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>27</v>
@@ -2656,7 +2655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>11641472</v>
       </c>
@@ -2672,19 +2671,19 @@
       <c r="E2" s="1">
         <v>10.499657768651609</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="2">
         <v>44090</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="2">
         <v>44109</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="K2" s="5">
@@ -2693,14 +2692,14 @@
       <c r="L2" s="5">
         <v>1</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>6537810</v>
       </c>
@@ -2716,19 +2715,19 @@
       <c r="E3" s="1">
         <v>16.659822039698838</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2">
         <v>44090</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="2">
         <v>44109</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>46</v>
       </c>
       <c r="K3" s="5">
@@ -2737,14 +2736,14 @@
       <c r="L3" s="5">
         <v>1</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>10273003</v>
       </c>
@@ -2760,17 +2759,17 @@
       <c r="E4" s="1">
         <v>9.2758384668035596</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="2">
         <v>44090</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>63</v>
       </c>
       <c r="K4" s="5">
@@ -2779,14 +2778,14 @@
       <c r="L4" s="5">
         <v>0</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4073694</v>
       </c>
@@ -2802,17 +2801,17 @@
       <c r="E5" s="1">
         <v>12.188911704312115</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="2">
         <v>44090</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>63</v>
       </c>
       <c r="K5" s="5">
@@ -2821,14 +2820,14 @@
       <c r="L5" s="5">
         <v>0</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>11578763</v>
       </c>
@@ -2844,19 +2843,19 @@
       <c r="E6" s="1">
         <v>10.234086242299794</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="2">
         <v>44090</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="2">
         <v>44105</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="5">
@@ -2865,10 +2864,10 @@
       <c r="L6" s="5">
         <v>1</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2885,25 +2884,25 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>12598894</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>8140425</v>
       </c>
@@ -3023,7 +3022,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>10160219</v>
       </c>
@@ -3061,7 +3060,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>7657294</v>
       </c>
@@ -3099,7 +3098,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6434087</v>
       </c>
@@ -3146,31 +3145,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE55476-AA2C-4AAE-B4AE-55AEF69223B1}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="82.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>86</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>27</v>
@@ -3223,7 +3222,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10721552</v>
       </c>
@@ -3245,16 +3244,16 @@
       <c r="G2" s="2">
         <v>44158</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>87</v>
       </c>
       <c r="J2" s="2">
         <v>44218</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="L2" s="2">
@@ -3263,20 +3262,20 @@
       <c r="M2" s="2">
         <v>44243</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>5358472</v>
       </c>
@@ -3298,34 +3297,34 @@
       <c r="G3" s="2">
         <v>44235</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>87</v>
       </c>
       <c r="J3" s="2">
         <v>44257</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>58</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O3" s="1">
         <v>1</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>14953858</v>
       </c>
@@ -3347,34 +3346,34 @@
       <c r="G4" s="2">
         <v>44235</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>87</v>
       </c>
       <c r="J4" s="2">
         <v>44257</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>58</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O4" s="1">
         <v>1</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>16036763</v>
       </c>
@@ -3396,16 +3395,16 @@
       <c r="G5" s="2">
         <v>43948</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>91</v>
       </c>
       <c r="J5" s="2">
         <v>44195</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>45</v>
       </c>
       <c r="L5" s="2">
@@ -3414,20 +3413,20 @@
       <c r="M5" s="2">
         <v>44200</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="Q5" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9396243</v>
       </c>
@@ -3449,16 +3448,16 @@
       <c r="G6" s="2">
         <v>43948</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>91</v>
       </c>
       <c r="J6" s="2">
         <v>44195</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>45</v>
       </c>
       <c r="L6" s="2">
@@ -3467,20 +3466,20 @@
       <c r="M6" s="2">
         <v>44200</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11811692</v>
       </c>
@@ -3502,16 +3501,16 @@
       <c r="G7" s="2">
         <v>43641</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>91</v>
       </c>
       <c r="J7" s="2">
         <v>44099</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>45</v>
       </c>
       <c r="L7" s="2">
@@ -3520,20 +3519,20 @@
       <c r="M7" s="2">
         <v>44091</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="Q7" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6913085</v>
       </c>
@@ -3555,16 +3554,16 @@
       <c r="G8" s="2">
         <v>43641</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>91</v>
       </c>
       <c r="J8" s="2">
         <v>44099</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>45</v>
       </c>
       <c r="L8" s="2">
@@ -3573,16 +3572,16 @@
       <c r="M8" s="2">
         <v>44091</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="7" t="s">
         <v>45</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="Q8" s="7" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3597,9 +3596,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3615,25 +3614,25 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" t="s">
         <v>97</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" t="s">
         <v>99</v>
       </c>
       <c r="M1" s="6" t="s">
@@ -3654,56 +3653,56 @@
       <c r="R1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>106</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" t="s">
         <v>108</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" t="s">
         <v>109</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" t="s">
         <v>110</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" t="s">
         <v>111</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" t="s">
         <v>112</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" t="s">
         <v>113</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" t="s">
         <v>114</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" t="s">
         <v>115</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" t="s">
         <v>116</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" t="s">
         <v>117</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" t="s">
         <v>118</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" t="s">
         <v>119</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1761444</v>
       </c>
@@ -3725,7 +3724,7 @@
       <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="9">
         <v>40031</v>
       </c>
       <c r="I2" t="s">
@@ -3734,29 +3733,29 @@
       <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>40371</v>
       </c>
       <c r="L2" t="s">
         <v>120</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <v>44208</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="9">
         <v>44202</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10">
+      <c r="O2" s="9"/>
+      <c r="P2" s="9">
         <v>44208</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="9">
         <v>43978</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="9">
         <v>43847</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="8">
         <v>1</v>
       </c>
       <c r="T2" s="4"/>
@@ -3775,14 +3774,14 @@
       <c r="AB2" t="s">
         <v>124</v>
       </c>
-      <c r="AC2" s="11">
+      <c r="AC2" s="10">
         <v>0</v>
       </c>
-      <c r="AD2" s="11">
+      <c r="AD2" s="10">
         <v>0</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
       <c r="AG2" t="s">
         <v>48</v>
       </c>
@@ -3790,7 +3789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1373595</v>
       </c>
@@ -3812,7 +3811,7 @@
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>40031</v>
       </c>
       <c r="I3" t="s">
@@ -3821,29 +3820,29 @@
       <c r="J3" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>40371</v>
       </c>
       <c r="L3" t="s">
         <v>126</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <v>44208</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>44249</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10">
+      <c r="O3" s="9"/>
+      <c r="P3" s="9">
         <v>44208</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="9">
         <v>43978</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>43847</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="8">
         <v>1</v>
       </c>
       <c r="T3" s="4"/>
@@ -3862,14 +3861,14 @@
       <c r="AB3" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" s="11">
+      <c r="AC3" s="10">
         <v>0</v>
       </c>
-      <c r="AD3" s="11">
+      <c r="AD3" s="10">
         <v>0</v>
       </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
       <c r="AG3" t="s">
         <v>48</v>
       </c>
@@ -3877,7 +3876,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>14065184</v>
       </c>
@@ -3899,7 +3898,7 @@
       <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>41894</v>
       </c>
       <c r="I4" t="s">
@@ -3908,29 +3907,29 @@
       <c r="J4" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>42235</v>
       </c>
       <c r="L4" t="s">
         <v>126</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>44173</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <v>44216</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10">
+      <c r="O4" s="9"/>
+      <c r="P4" s="9">
         <v>43837</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="9">
         <v>44109</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="9">
         <v>44116</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="8">
         <v>1</v>
       </c>
       <c r="T4" s="4"/>
@@ -3949,14 +3948,14 @@
       <c r="AB4" t="s">
         <v>133</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AC4" s="10">
         <v>0</v>
       </c>
-      <c r="AD4" s="11">
+      <c r="AD4" s="10">
         <v>0</v>
       </c>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
       <c r="AG4" t="s">
         <v>48</v>
       </c>
@@ -3964,7 +3963,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2529037</v>
       </c>
@@ -3986,7 +3985,7 @@
       <c r="G5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>40233</v>
       </c>
       <c r="I5" t="s">
@@ -3995,29 +3994,29 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>41169</v>
       </c>
       <c r="L5" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>44253</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <v>44249</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10">
+      <c r="O5" s="9"/>
+      <c r="P5" s="9">
         <v>44253</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="9">
         <v>44047</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="9">
         <v>43815</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="8">
         <v>2</v>
       </c>
       <c r="T5" s="4"/>
@@ -4033,14 +4032,14 @@
       <c r="AB5" t="s">
         <v>124</v>
       </c>
-      <c r="AC5" s="11">
+      <c r="AC5" s="10">
         <v>0</v>
       </c>
-      <c r="AD5" s="11">
+      <c r="AD5" s="10">
         <v>0</v>
       </c>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
       <c r="AG5" t="s">
         <v>135</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3623204</v>
       </c>
@@ -4070,7 +4069,7 @@
       <c r="G6" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>39743</v>
       </c>
       <c r="I6" t="s">
@@ -4079,32 +4078,32 @@
       <c r="J6" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>40021</v>
       </c>
       <c r="L6" t="s">
         <v>138</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>44055</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <v>44050</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10">
+      <c r="O6" s="9"/>
+      <c r="P6" s="9">
         <v>44055</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="9">
         <v>44004</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="9">
         <v>44057</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="8">
         <v>1</v>
       </c>
-      <c r="T6" s="10">
+      <c r="T6" s="9">
         <v>44096</v>
       </c>
       <c r="U6" t="s">
@@ -4125,14 +4124,14 @@
       <c r="AB6" t="s">
         <v>124</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6" s="10">
         <v>0</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AD6" s="10">
         <v>0</v>
       </c>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
       <c r="AG6" t="s">
         <v>50</v>
       </c>
@@ -4153,9 +4152,9 @@
       <selection sqref="A1:M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4196,7 +4195,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7961370</v>
       </c>
@@ -4237,7 +4236,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10414520</v>
       </c>
@@ -4278,7 +4277,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>13782635</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4939073</v>
       </c>
@@ -4360,7 +4359,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6102196</v>
       </c>
@@ -4401,7 +4400,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2295089</v>
       </c>

</xml_diff>